<commit_message>
Rename TestJframe to GUIPrototype Changed Backlog
</commit_message>
<xml_diff>
--- a/src/doc/Backlog.xlsx
+++ b/src/doc/Backlog.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>12h</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Design GUI Prototype</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -470,7 +482,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,6 +527,9 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -603,7 +618,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,28 +671,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="G2" t="s">
         <v>6</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
@@ -691,16 +708,16 @@
         <v>5</v>
       </c>
       <c r="H3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
@@ -714,17 +731,16 @@
         <v>5</v>
       </c>
       <c r="H4">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <f>SUM(I4:I4)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
@@ -738,16 +754,16 @@
         <v>7</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
@@ -761,16 +777,16 @@
         <v>5</v>
       </c>
       <c r="H6">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added GraphPanel to MainGUI
</commit_message>
<xml_diff>
--- a/src/doc/Backlog.xlsx
+++ b/src/doc/Backlog.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -113,9 +113,6 @@
     <t>open</t>
   </si>
   <si>
-    <t>in progress</t>
-  </si>
-  <si>
     <t>Vertex Component</t>
   </si>
   <si>
@@ -153,6 +150,18 @@
   </si>
   <si>
     <t>gugec1</t>
+  </si>
+  <si>
+    <t>in Progess</t>
+  </si>
+  <si>
+    <t>Edge Format</t>
+  </si>
+  <si>
+    <t>Vertex Format</t>
+  </si>
+  <si>
+    <t>in Progress</t>
   </si>
 </sst>
 </file>
@@ -651,10 +660,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,10 +724,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -730,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
@@ -741,10 +750,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -767,10 +776,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -793,10 +802,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -819,10 +828,10 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -834,35 +843,57 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>